<commit_message>
add some more tests
</commit_message>
<xml_diff>
--- a/testset/C2PA-JPT Testfiles.xlsx
+++ b/testset/C2PA-JPT Testfiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/lrosenth_adobe_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/Development/c2pa-testfile-maker/testset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="8_{A3E98B81-6F37-5C48-BFFA-8BC1DB833127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4EE9772-4A9F-6248-BAE7-58B9E16CFFDC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59F45F4-8BD4-7A4D-B1E8-C6251C2ABB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="71200" yWindow="8000" windowWidth="30080" windowHeight="25840" xr2:uid="{8EA77C23-A43E-9342-9FFB-5C3237DC0EFB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="67">
   <si>
     <t>Test Type</t>
   </si>
@@ -289,10 +289,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,19 +635,19 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7" style="3" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -663,12 +662,12 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B2" t="s">
@@ -682,7 +681,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B3" t="s">
@@ -702,7 +701,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
@@ -722,7 +721,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
@@ -742,7 +741,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B6" t="s">
@@ -762,7 +761,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B7" t="s">
@@ -782,7 +781,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B8" t="s">
@@ -796,7 +795,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B9" t="s">
@@ -816,7 +815,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B10" t="s">
@@ -836,7 +835,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B11" t="s">
@@ -856,7 +855,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B12" t="s">
@@ -876,6 +875,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -890,7 +892,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B14" t="s">
@@ -907,7 +909,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B15" t="s">
@@ -952,7 +954,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B18" t="s">
@@ -966,7 +968,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B19" t="s">
@@ -980,7 +982,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B20" t="s">
@@ -1000,7 +1002,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B21" t="s">
@@ -1020,7 +1022,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="s">
@@ -1040,7 +1042,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B23" t="s">
@@ -1060,7 +1062,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B24" t="s">
@@ -1080,7 +1082,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B25" t="s">
@@ -1117,7 +1119,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B27" t="s">
@@ -1137,7 +1139,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B28" t="s">
@@ -1174,7 +1176,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B30" t="s">
@@ -1191,7 +1193,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B31" t="s">
@@ -1208,7 +1210,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B32" t="s">
@@ -1225,7 +1227,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B33" t="s">
@@ -1312,7 +1314,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B41" t="s">

</xml_diff>

<commit_message>
Added new tests for action templates and related actions
</commit_message>
<xml_diff>
--- a/testset/C2PA-JPT Testfiles.xlsx
+++ b/testset/C2PA-JPT Testfiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/Development/c2pa-testfile-maker/testset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59F45F4-8BD4-7A4D-B1E8-C6251C2ABB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38065CF4-47A6-C44A-A781-78AD2A5EA626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="71200" yWindow="8000" windowWidth="30080" windowHeight="25840" xr2:uid="{8EA77C23-A43E-9342-9FFB-5C3237DC0EFB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="68">
   <si>
     <t>Test Type</t>
   </si>
@@ -125,9 +125,6 @@
     <t>templates</t>
   </si>
   <si>
-    <t>need various template tests</t>
-  </si>
-  <si>
     <t>icon</t>
   </si>
   <si>
@@ -237,6 +234,12 @@
   </si>
   <si>
     <t>custom metadata on c2pa.placed (w/ activeManifest)</t>
+  </si>
+  <si>
+    <t>simple template</t>
+  </si>
+  <si>
+    <t>special "all" template</t>
   </si>
 </sst>
 </file>
@@ -632,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1249C59-3BE9-8E43-B865-F2FCA3C2B265}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,7 +651,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -657,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -668,7 +671,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -682,7 +685,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -691,18 +694,18 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -711,18 +714,18 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -731,18 +734,18 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -751,18 +754,18 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -771,7 +774,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -782,7 +785,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -796,7 +799,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -805,18 +808,18 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -825,18 +828,18 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -845,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -856,7 +859,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -865,7 +868,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -876,7 +879,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -893,7 +896,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -910,7 +913,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -933,10 +936,10 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
         <v>30</v>
-      </c>
-      <c r="F16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -947,15 +950,15 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -969,7 +972,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -983,7 +986,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -992,18 +995,18 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1012,18 +1015,18 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -1032,18 +1035,18 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="s">
         <v>64</v>
-      </c>
-      <c r="F22" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -1052,18 +1055,18 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -1072,18 +1075,18 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -1092,13 +1095,13 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1109,18 +1112,18 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -1129,18 +1132,18 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -1149,7 +1152,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
         <v>9</v>
@@ -1166,18 +1169,18 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1194,7 +1197,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -1211,7 +1214,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -1228,7 +1231,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -1244,6 +1247,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
@@ -1254,10 +1260,13 @@
         <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -1265,10 +1274,10 @@
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1279,10 +1288,10 @@
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1293,38 +1302,55 @@
         <v>5</v>
       </c>
       <c r="E37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" t="s">
         <v>34</v>
       </c>
-      <c r="F37" t="s">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="F39" t="s">
         <v>36</v>
       </c>
-      <c r="F38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" t="s">
         <v>62</v>
-      </c>
-      <c r="F41" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>